<commit_message>
added my rxia directory
</commit_message>
<xml_diff>
--- a/Personal/Divident Strat/CoveredCallsETN.xlsx
+++ b/Personal/Divident Strat/CoveredCallsETN.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RedX Capital\Divident Strat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RedXCapital\Personal\Divident Strat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E07DBC48-FEA3-4398-83FA-4A49BF811723}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A495E0B-3A33-45C7-924C-B0B12BFB2DFF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B9E2AEA3-BDB3-4DF6-A026-E66CF7C351FF}"/>
   </bookViews>
@@ -17,6 +17,9 @@
     <sheet name="USOI" sheetId="3" r:id="rId2"/>
     <sheet name="MVLR" sheetId="2" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">REML!$A$5:$F$65</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>Date</t>
   </si>
@@ -35,169 +38,7 @@
     <t>Dividends</t>
   </si>
   <si>
-    <t>0.207 Dividend</t>
-  </si>
-  <si>
-    <t>0.031 Dividend</t>
-  </si>
-  <si>
-    <t>0.057 Dividend</t>
-  </si>
-  <si>
-    <t>0.204 Dividend</t>
-  </si>
-  <si>
-    <t>0.054 Dividend</t>
-  </si>
-  <si>
-    <t>0.194 Dividend</t>
-  </si>
-  <si>
-    <t>0.018 Dividend</t>
-  </si>
-  <si>
-    <t>0.02 Dividend</t>
-  </si>
-  <si>
-    <t>0.193 Dividend</t>
-  </si>
-  <si>
-    <t>0.022 Dividend</t>
-  </si>
-  <si>
-    <t>0.035 Dividend</t>
-  </si>
-  <si>
-    <t>0.144 Dividend</t>
-  </si>
-  <si>
-    <t>0.021 Dividend</t>
-  </si>
-  <si>
-    <t>0.028 Dividend</t>
-  </si>
-  <si>
-    <t>0.124 Dividend</t>
-  </si>
-  <si>
-    <t>0.025 Dividend</t>
-  </si>
-  <si>
-    <t>0.169 Dividend</t>
-  </si>
-  <si>
-    <t>0.092 Dividend</t>
-  </si>
-  <si>
-    <t>0.068 Dividend</t>
-  </si>
-  <si>
-    <t>1.009 Dividend</t>
-  </si>
-  <si>
-    <t>0.244 Dividend</t>
-  </si>
-  <si>
-    <t>0.775 Dividend</t>
-  </si>
-  <si>
-    <t>0.088 Dividend</t>
-  </si>
-  <si>
-    <t>0.126 Dividend</t>
-  </si>
-  <si>
-    <t>0.923 Dividend</t>
-  </si>
-  <si>
-    <t>0.095 Dividend</t>
-  </si>
-  <si>
-    <t>0.236 Dividend</t>
-  </si>
-  <si>
-    <t>0.952 Dividend</t>
-  </si>
-  <si>
     <t>0.09 Dividend</t>
-  </si>
-  <si>
-    <t>0.07 Dividend</t>
-  </si>
-  <si>
-    <t>1.154 Dividend</t>
-  </si>
-  <si>
-    <t>0.102 Dividend</t>
-  </si>
-  <si>
-    <t>0.145 Dividend</t>
-  </si>
-  <si>
-    <t>1.077 Dividend</t>
-  </si>
-  <si>
-    <t>0.114 Dividend</t>
-  </si>
-  <si>
-    <t>0.159 Dividend</t>
-  </si>
-  <si>
-    <t>1.138 Dividend</t>
-  </si>
-  <si>
-    <t>0.086 Dividend</t>
-  </si>
-  <si>
-    <t>0.119 Dividend</t>
-  </si>
-  <si>
-    <t>1.088 Dividend</t>
-  </si>
-  <si>
-    <t>0.065 Dividend</t>
-  </si>
-  <si>
-    <t>0.071 Dividend</t>
-  </si>
-  <si>
-    <t>1.27 Dividend</t>
-  </si>
-  <si>
-    <t>0.078 Dividend</t>
-  </si>
-  <si>
-    <t>0.147 Dividend</t>
-  </si>
-  <si>
-    <t>1.258 Dividend</t>
-  </si>
-  <si>
-    <t>0.081 Dividend</t>
-  </si>
-  <si>
-    <t>1.224 Dividend</t>
-  </si>
-  <si>
-    <t>0.087 Dividend</t>
-  </si>
-  <si>
-    <t>0.138 Dividend</t>
-  </si>
-  <si>
-    <t>1.214 Dividend</t>
-  </si>
-  <si>
-    <t>0.069 Dividend</t>
-  </si>
-  <si>
-    <t>0.077 Dividend</t>
-  </si>
-  <si>
-    <t>1.233 Dividend</t>
-  </si>
-  <si>
-    <t>0.149 Dividend</t>
   </si>
   <si>
     <t>REML</t>
@@ -253,6 +94,30 @@
   <si>
     <t>USOI</t>
   </si>
+  <si>
+    <t>DAY</t>
+  </si>
+  <si>
+    <t>AVERAGE</t>
+  </si>
+  <si>
+    <t>MONTH</t>
+  </si>
+  <si>
+    <t>Avg Covid Dividends</t>
+  </si>
+  <si>
+    <t>Avg Dividends</t>
+  </si>
+  <si>
+    <t>Year Minus Fees</t>
+  </si>
+  <si>
+    <t>ROI</t>
+  </si>
+  <si>
+    <t>DayOfWeek</t>
+  </si>
 </sst>
 </file>
 
@@ -260,7 +125,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="168" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -303,7 +168,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1831,782 +1696,1452 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A3025FD-7082-4C39-8F16-925749F0F888}">
-  <dimension ref="A1:I62"/>
+  <dimension ref="A1:L65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>44482</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="6">
-        <v>0.20699999999999999</v>
-      </c>
-      <c r="D3">
-        <f>AVERAGE(C3:C22)</f>
+        <v>24</v>
+      </c>
+      <c r="C2">
+        <f>AVERAGE(B6:B25)</f>
         <v>8.4350000000000008E-2</v>
       </c>
-      <c r="E3" s="7">
-        <f>D3/7.41</f>
+      <c r="D2" s="7">
+        <f>C2/7.41</f>
         <v>1.1383265856950068E-2</v>
       </c>
-      <c r="F3" s="6">
-        <f>(E3+1)^12-0.005</f>
+      <c r="E2" s="6">
+        <f>(D2+1)^12-0.005</f>
         <v>1.1404843584441409</v>
       </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>44452</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="6">
-        <v>3.1E-2</v>
-      </c>
-      <c r="D4">
-        <f>AVERAGE(C3:C62)</f>
-        <v>0.31703333333333344</v>
-      </c>
-      <c r="E4" s="7">
-        <f>D4/7.41</f>
-        <v>4.2784525416104377E-2</v>
-      </c>
-      <c r="F4" s="6">
-        <f>(E4+1)^12</f>
-        <v>1.653236302169699</v>
-      </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>44419</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="6">
-        <v>5.7000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>44390</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="6">
-        <v>0.20399999999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>44357</v>
-      </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="6">
-        <v>3.1E-2</v>
-      </c>
-      <c r="D7">
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2">
         <f>33.41/7.4-1</f>
         <v>3.5148648648648644</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3">
+        <f>AVERAGE(B6:B65)</f>
+        <v>0.31703333333333344</v>
+      </c>
+      <c r="D3" s="7">
+        <f>C3/7.41</f>
+        <v>4.2784525416104377E-2</v>
+      </c>
+      <c r="E3" s="6">
+        <f>(D3+1)^12</f>
+        <v>1.653236302169699</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>44482</v>
+      </c>
+      <c r="B6" s="6">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="C6" t="str">
+        <f>TEXT(A6,"ddd")</f>
+        <v>Wed</v>
+      </c>
+      <c r="D6" s="6" t="str">
+        <f>TEXT(A6,"mmm")</f>
+        <v>Oct</v>
+      </c>
+      <c r="E6" s="6">
+        <f t="shared" ref="E6:E37" si="0">DAY(A6)</f>
+        <v>13</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ref="F6:F23" si="1">AVERAGE(E6,E18,E30,E42,E54)</f>
+        <v>11.8</v>
+      </c>
+      <c r="K6" s="2"/>
+      <c r="L6" s="3"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>44452</v>
+      </c>
+      <c r="B7" s="6">
+        <v>3.1E-2</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" ref="C7:C65" si="2">TEXT(A7,"ddd")</f>
+        <v>Mon</v>
+      </c>
+      <c r="D7" s="6" t="str">
+        <f t="shared" ref="D7:D65" si="3">TEXT(A7,"mmm")</f>
+        <v>Sep</v>
+      </c>
+      <c r="E7" s="6">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>12.4</v>
+      </c>
+      <c r="K7" s="2"/>
+      <c r="L7" s="3"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
+        <v>44419</v>
+      </c>
+      <c r="B8" s="6">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="2"/>
+        <v>Wed</v>
+      </c>
+      <c r="D8" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Aug</v>
+      </c>
+      <c r="E8" s="6">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>44390</v>
+      </c>
+      <c r="B9" s="6">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="2"/>
+        <v>Tue</v>
+      </c>
+      <c r="D9" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Jul</v>
+      </c>
+      <c r="E9" s="6">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>11.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>44357</v>
+      </c>
+      <c r="B10" s="6">
+        <v>3.1E-2</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="2"/>
+        <v>Thu</v>
+      </c>
+      <c r="D10" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Jun</v>
+      </c>
+      <c r="E10" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>10.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <v>44328</v>
       </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="6">
+      <c r="B11" s="6">
         <v>5.3999999999999999E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+      <c r="C11" t="str">
+        <f t="shared" si="2"/>
+        <v>Wed</v>
+      </c>
+      <c r="D11" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>May</v>
+      </c>
+      <c r="E11" s="6">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>10.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <v>44298</v>
       </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="6">
+      <c r="B12" s="6">
         <v>0.19400000000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+      <c r="C12" t="str">
+        <f t="shared" si="2"/>
+        <v>Mon</v>
+      </c>
+      <c r="D12" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Apr</v>
+      </c>
+      <c r="E12" s="6">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>10.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
         <v>44265</v>
       </c>
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="6">
+      <c r="B13" s="6">
         <v>1.7999999999999999E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+      <c r="C13" t="str">
+        <f t="shared" si="2"/>
+        <v>Wed</v>
+      </c>
+      <c r="D13" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Mar</v>
+      </c>
+      <c r="E13" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
         <v>44237</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B14" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="2"/>
+        <v>Wed</v>
+      </c>
+      <c r="D14" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Feb</v>
+      </c>
+      <c r="E14" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>44209</v>
+      </c>
+      <c r="B15" s="6">
+        <v>0.193</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="2"/>
+        <v>Wed</v>
+      </c>
+      <c r="D15" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Jan</v>
+      </c>
+      <c r="E15" s="6">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>11.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>44175</v>
+      </c>
+      <c r="B16" s="6">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="2"/>
+        <v>Thu</v>
+      </c>
+      <c r="D16" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Dec</v>
+      </c>
+      <c r="E16" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>44147</v>
+      </c>
+      <c r="B17" s="6">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="2"/>
+        <v>Thu</v>
+      </c>
+      <c r="D17" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Nov</v>
+      </c>
+      <c r="E17" s="6">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>11.4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>44117</v>
+      </c>
+      <c r="B18" s="6">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="2"/>
+        <v>Tue</v>
+      </c>
+      <c r="D18" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Oct</v>
+      </c>
+      <c r="E18" s="6">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>44085</v>
+      </c>
+      <c r="B19" s="6">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="2"/>
+        <v>Fri</v>
+      </c>
+      <c r="D19" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Sep</v>
+      </c>
+      <c r="E19" s="6">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>12.25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>44055</v>
+      </c>
+      <c r="B20" s="6">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="2"/>
+        <v>Wed</v>
+      </c>
+      <c r="D20" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Aug</v>
+      </c>
+      <c r="E20" s="6">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>10.75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>44022</v>
+      </c>
+      <c r="B21" s="6">
+        <v>0.124</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="2"/>
+        <v>Fri</v>
+      </c>
+      <c r="D21" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Jul</v>
+      </c>
+      <c r="E21" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="1"/>
+        <v>11.25</v>
+      </c>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>43992</v>
+      </c>
+      <c r="B22" s="6">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="2"/>
+        <v>Wed</v>
+      </c>
+      <c r="D22" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Jun</v>
+      </c>
+      <c r="E22" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="1"/>
+        <v>10.75</v>
+      </c>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>43963</v>
+      </c>
+      <c r="B23" s="6">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="2"/>
+        <v>Tue</v>
+      </c>
+      <c r="D23" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>May</v>
+      </c>
+      <c r="E23" s="6">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="1"/>
+        <v>10.25</v>
+      </c>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B24" s="6">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="2"/>
+        <v>Thu</v>
+      </c>
+      <c r="D24" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Apr</v>
+      </c>
+      <c r="E24" s="6">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C11" s="5">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>44209</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="F24">
+        <f t="shared" ref="F24" si="4">AVERAGE(E24,E36,E48,E60,E72)</f>
         <v>10</v>
       </c>
-      <c r="C12" s="6">
-        <v>0.193</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>44175</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>43901</v>
+      </c>
+      <c r="B25" s="6">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="2"/>
+        <v>Wed</v>
+      </c>
+      <c r="D25" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Mar</v>
+      </c>
+      <c r="E25" s="6">
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C13" s="6">
-        <v>2.1999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>44147</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="F25">
+        <f t="shared" ref="F25:F30" si="5">AVERAGE(E25,E37,E49,E61,E73)</f>
+        <v>11</v>
+      </c>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>43873</v>
+      </c>
+      <c r="B26" s="6">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="2"/>
+        <v>Wed</v>
+      </c>
+      <c r="D26" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Feb</v>
+      </c>
+      <c r="E26" s="6">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C14" s="6">
-        <v>3.5000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>44117</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="F26">
+        <f t="shared" si="5"/>
+        <v>11.25</v>
+      </c>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>43843</v>
+      </c>
+      <c r="B27" s="6">
+        <v>1.0089999999999999</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="2"/>
+        <v>Mon</v>
+      </c>
+      <c r="D27" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Jan</v>
+      </c>
+      <c r="E27" s="6">
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C15" s="6">
-        <v>0.14399999999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>44085</v>
-      </c>
-      <c r="B16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="6">
-        <v>2.1000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>44055</v>
-      </c>
-      <c r="B17" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="6">
-        <v>2.8000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>44022</v>
-      </c>
-      <c r="B18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="6">
-        <v>0.124</v>
-      </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>43992</v>
-      </c>
-      <c r="B19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="6">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>43963</v>
-      </c>
-      <c r="B20" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="6">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>43930</v>
-      </c>
-      <c r="B21" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="6">
-        <v>0.16900000000000001</v>
-      </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>43901</v>
-      </c>
-      <c r="B22" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="6">
+      <c r="F27">
+        <f t="shared" si="5"/>
+        <v>11.5</v>
+      </c>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>43810</v>
+      </c>
+      <c r="B28" s="6">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>43873</v>
-      </c>
-      <c r="B23" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="6">
-        <v>6.8000000000000005E-2</v>
-      </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>43843</v>
-      </c>
-      <c r="B24" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="6">
-        <v>1.0089999999999999</v>
-      </c>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>43810</v>
-      </c>
-      <c r="B25" t="s">
-        <v>19</v>
-      </c>
-      <c r="C25" s="6">
-        <v>9.1999999999999998E-2</v>
-      </c>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
+      <c r="C28" t="str">
+        <f t="shared" si="2"/>
+        <v>Wed</v>
+      </c>
+      <c r="D28" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Dec</v>
+      </c>
+      <c r="E28" s="6">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
         <v>43782</v>
       </c>
-      <c r="B26" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" s="6">
+      <c r="B29" s="6">
         <v>0.24399999999999999</v>
       </c>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
+      <c r="C29" t="str">
+        <f t="shared" si="2"/>
+        <v>Wed</v>
+      </c>
+      <c r="D29" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Nov</v>
+      </c>
+      <c r="E29" s="6">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="5"/>
+        <v>11.25</v>
+      </c>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
         <v>43748</v>
       </c>
-      <c r="B27" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" s="6">
+      <c r="B30" s="6">
         <v>0.77500000000000002</v>
       </c>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
+      <c r="C30" t="str">
+        <f t="shared" si="2"/>
+        <v>Thu</v>
+      </c>
+      <c r="D30" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Oct</v>
+      </c>
+      <c r="E30" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
         <v>43720</v>
       </c>
-      <c r="B28" t="s">
-        <v>24</v>
-      </c>
-      <c r="C28" s="6">
+      <c r="B31" s="6">
         <v>8.7999999999999995E-2</v>
       </c>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
+      <c r="C31" t="str">
+        <f t="shared" si="2"/>
+        <v>Thu</v>
+      </c>
+      <c r="D31" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Sep</v>
+      </c>
+      <c r="E31" s="6">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
         <v>43689</v>
       </c>
-      <c r="B29" t="s">
-        <v>25</v>
-      </c>
-      <c r="C29" s="6">
+      <c r="B32" s="6">
         <v>0.126</v>
       </c>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
+      <c r="C32" t="str">
+        <f t="shared" si="2"/>
+        <v>Mon</v>
+      </c>
+      <c r="D32" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Aug</v>
+      </c>
+      <c r="E32" s="6">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
         <v>43657</v>
       </c>
-      <c r="B30" t="s">
-        <v>26</v>
-      </c>
-      <c r="C30" s="6">
+      <c r="B33" s="6">
         <v>0.92300000000000004</v>
       </c>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
+      <c r="C33" t="str">
+        <f t="shared" si="2"/>
+        <v>Thu</v>
+      </c>
+      <c r="D33" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Jul</v>
+      </c>
+      <c r="E33" s="6">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
         <v>43628</v>
       </c>
-      <c r="B31" t="s">
-        <v>27</v>
-      </c>
-      <c r="C31" s="6">
+      <c r="B34" s="6">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
+      <c r="C34" t="str">
+        <f t="shared" si="2"/>
+        <v>Wed</v>
+      </c>
+      <c r="D34" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Jun</v>
+      </c>
+      <c r="E34" s="6">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
         <v>43595</v>
       </c>
-      <c r="B32" t="s">
-        <v>28</v>
-      </c>
-      <c r="C32" s="6">
+      <c r="B35" s="6">
         <v>0.23599999999999999</v>
       </c>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
+      <c r="C35" t="str">
+        <f t="shared" si="2"/>
+        <v>Fri</v>
+      </c>
+      <c r="D35" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>May</v>
+      </c>
+      <c r="E35" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
         <v>43565</v>
       </c>
-      <c r="B33" t="s">
-        <v>29</v>
-      </c>
-      <c r="C33" s="6">
+      <c r="B36" s="6">
         <v>0.95199999999999996</v>
       </c>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
+      <c r="C36" t="str">
+        <f t="shared" si="2"/>
+        <v>Wed</v>
+      </c>
+      <c r="D36" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Apr</v>
+      </c>
+      <c r="E36" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
         <v>43536</v>
       </c>
-      <c r="B34" t="s">
-        <v>30</v>
-      </c>
-      <c r="C34" s="5">
+      <c r="B37" s="5">
         <v>0.09</v>
       </c>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
+      <c r="C37" t="str">
+        <f t="shared" si="2"/>
+        <v>Tue</v>
+      </c>
+      <c r="D37" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Mar</v>
+      </c>
+      <c r="E37" s="6">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
         <v>43508</v>
       </c>
-      <c r="B35" t="s">
-        <v>31</v>
-      </c>
-      <c r="C35" s="5">
+      <c r="B38" s="5">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="4">
+      <c r="C38" t="str">
+        <f t="shared" si="2"/>
+        <v>Tue</v>
+      </c>
+      <c r="D38" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Feb</v>
+      </c>
+      <c r="E38" s="6">
+        <f t="shared" ref="E38:E65" si="6">DAY(A38)</f>
+        <v>12</v>
+      </c>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
         <v>43476</v>
       </c>
-      <c r="B36" t="s">
-        <v>32</v>
-      </c>
-      <c r="C36" s="6">
+      <c r="B39" s="6">
         <v>1.1539999999999999</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="4">
+      <c r="C39" t="str">
+        <f t="shared" si="2"/>
+        <v>Fri</v>
+      </c>
+      <c r="D39" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Jan</v>
+      </c>
+      <c r="E39" s="6">
+        <f t="shared" si="6"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
         <v>43446</v>
       </c>
-      <c r="B37" t="s">
-        <v>33</v>
-      </c>
-      <c r="C37" s="6">
+      <c r="B40" s="6">
         <v>0.10199999999999999</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="4">
+      <c r="C40" t="str">
+        <f t="shared" si="2"/>
+        <v>Wed</v>
+      </c>
+      <c r="D40" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Dec</v>
+      </c>
+      <c r="E40" s="6">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
         <v>43417</v>
       </c>
-      <c r="B38" t="s">
-        <v>34</v>
-      </c>
-      <c r="C38" s="6">
+      <c r="B41" s="6">
         <v>0.14499999999999999</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="4">
+      <c r="C41" t="str">
+        <f t="shared" si="2"/>
+        <v>Tue</v>
+      </c>
+      <c r="D41" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Nov</v>
+      </c>
+      <c r="E41" s="6">
+        <f t="shared" si="6"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
         <v>43384</v>
       </c>
-      <c r="B39" t="s">
-        <v>35</v>
-      </c>
-      <c r="C39" s="6">
+      <c r="B42" s="6">
         <v>1.077</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="4">
+      <c r="C42" t="str">
+        <f t="shared" si="2"/>
+        <v>Thu</v>
+      </c>
+      <c r="D42" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Oct</v>
+      </c>
+      <c r="E42" s="6">
+        <f t="shared" si="6"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
         <v>43356</v>
       </c>
-      <c r="B40" t="s">
-        <v>36</v>
-      </c>
-      <c r="C40" s="6">
+      <c r="B43" s="6">
         <v>0.114</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="4">
+      <c r="C43" t="str">
+        <f t="shared" si="2"/>
+        <v>Thu</v>
+      </c>
+      <c r="D43" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Sep</v>
+      </c>
+      <c r="E43" s="6">
+        <f t="shared" si="6"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
         <v>43322</v>
       </c>
-      <c r="B41" t="s">
-        <v>37</v>
-      </c>
-      <c r="C41" s="6">
+      <c r="B44" s="6">
         <v>0.159</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="4">
+      <c r="C44" t="str">
+        <f t="shared" si="2"/>
+        <v>Fri</v>
+      </c>
+      <c r="D44" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Aug</v>
+      </c>
+      <c r="E44" s="6">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
         <v>43293</v>
       </c>
-      <c r="B42" t="s">
-        <v>38</v>
-      </c>
-      <c r="C42" s="6">
+      <c r="B45" s="6">
         <v>1.1379999999999999</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="4">
+      <c r="C45" t="str">
+        <f t="shared" si="2"/>
+        <v>Thu</v>
+      </c>
+      <c r="D45" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Jul</v>
+      </c>
+      <c r="E45" s="6">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
         <v>43263</v>
       </c>
-      <c r="B43" t="s">
-        <v>39</v>
-      </c>
-      <c r="C43" s="6">
+      <c r="B46" s="6">
         <v>8.5999999999999993E-2</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="4">
+      <c r="C46" t="str">
+        <f t="shared" si="2"/>
+        <v>Tue</v>
+      </c>
+      <c r="D46" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Jun</v>
+      </c>
+      <c r="E46" s="6">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
         <v>43230</v>
       </c>
-      <c r="B44" t="s">
-        <v>40</v>
-      </c>
-      <c r="C44" s="6">
+      <c r="B47" s="6">
         <v>0.11899999999999999</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="4">
+      <c r="C47" t="str">
+        <f t="shared" si="2"/>
+        <v>Thu</v>
+      </c>
+      <c r="D47" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>May</v>
+      </c>
+      <c r="E47" s="6">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
         <v>43200</v>
       </c>
-      <c r="B45" t="s">
-        <v>41</v>
-      </c>
-      <c r="C45" s="6">
+      <c r="B48" s="6">
         <v>1.0880000000000001</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="4">
+      <c r="C48" t="str">
+        <f t="shared" si="2"/>
+        <v>Tue</v>
+      </c>
+      <c r="D48" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Apr</v>
+      </c>
+      <c r="E48" s="6">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
         <v>43171</v>
       </c>
-      <c r="B46" t="s">
-        <v>42</v>
-      </c>
-      <c r="C46" s="6">
+      <c r="B49" s="6">
         <v>6.5000000000000002E-2</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="4">
+      <c r="C49" t="str">
+        <f t="shared" si="2"/>
+        <v>Mon</v>
+      </c>
+      <c r="D49" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Mar</v>
+      </c>
+      <c r="E49" s="6">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
         <v>43143</v>
       </c>
-      <c r="B47" t="s">
-        <v>43</v>
-      </c>
-      <c r="C47" s="6">
+      <c r="B50" s="6">
         <v>7.0999999999999994E-2</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="4">
+      <c r="C50" t="str">
+        <f t="shared" si="2"/>
+        <v>Mon</v>
+      </c>
+      <c r="D50" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Feb</v>
+      </c>
+      <c r="E50" s="6">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
         <v>43111</v>
       </c>
-      <c r="B48" t="s">
-        <v>44</v>
-      </c>
-      <c r="C48" s="5">
+      <c r="B51" s="5">
         <v>1.27</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="4">
+      <c r="C51" t="str">
+        <f t="shared" si="2"/>
+        <v>Thu</v>
+      </c>
+      <c r="D51" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Jan</v>
+      </c>
+      <c r="E51" s="6">
+        <f t="shared" si="6"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
         <v>43081</v>
       </c>
-      <c r="B49" t="s">
-        <v>45</v>
-      </c>
-      <c r="C49" s="6">
+      <c r="B52" s="6">
         <v>7.8E-2</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="4">
+      <c r="C52" t="str">
+        <f t="shared" si="2"/>
+        <v>Tue</v>
+      </c>
+      <c r="D52" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Dec</v>
+      </c>
+      <c r="E52" s="6">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
         <v>43049</v>
       </c>
-      <c r="B50" t="s">
-        <v>46</v>
-      </c>
-      <c r="C50" s="6">
+      <c r="B53" s="6">
         <v>0.14699999999999999</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="4">
+      <c r="C53" t="str">
+        <f t="shared" si="2"/>
+        <v>Fri</v>
+      </c>
+      <c r="D53" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Nov</v>
+      </c>
+      <c r="E53" s="6">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
         <v>43020</v>
       </c>
-      <c r="B51" t="s">
-        <v>47</v>
-      </c>
-      <c r="C51" s="6">
+      <c r="B54" s="6">
         <v>1.258</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="4">
+      <c r="C54" t="str">
+        <f t="shared" si="2"/>
+        <v>Thu</v>
+      </c>
+      <c r="D54" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Oct</v>
+      </c>
+      <c r="E54" s="6">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
         <v>42991</v>
       </c>
-      <c r="B52" t="s">
-        <v>48</v>
-      </c>
-      <c r="C52" s="6">
+      <c r="B55" s="6">
         <v>8.1000000000000003E-2</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="4">
+      <c r="C55" t="str">
+        <f t="shared" si="2"/>
+        <v>Wed</v>
+      </c>
+      <c r="D55" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Sep</v>
+      </c>
+      <c r="E55" s="6">
+        <f t="shared" si="6"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
         <v>42956</v>
       </c>
-      <c r="B53" t="s">
-        <v>46</v>
-      </c>
-      <c r="C53" s="6">
+      <c r="B56" s="6">
         <v>0.14699999999999999</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="4">
+      <c r="C56" t="str">
+        <f t="shared" si="2"/>
+        <v>Wed</v>
+      </c>
+      <c r="D56" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Aug</v>
+      </c>
+      <c r="E56" s="6">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
         <v>42928</v>
       </c>
-      <c r="B54" t="s">
-        <v>49</v>
-      </c>
-      <c r="C54" s="6">
+      <c r="B57" s="6">
         <v>1.224</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="4">
+      <c r="C57" t="str">
+        <f t="shared" si="2"/>
+        <v>Wed</v>
+      </c>
+      <c r="D57" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Jul</v>
+      </c>
+      <c r="E57" s="6">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
         <v>42895</v>
       </c>
-      <c r="B55" t="s">
-        <v>50</v>
-      </c>
-      <c r="C55" s="6">
+      <c r="B58" s="6">
         <v>8.6999999999999994E-2</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="4">
+      <c r="C58" t="str">
+        <f t="shared" si="2"/>
+        <v>Fri</v>
+      </c>
+      <c r="D58" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Jun</v>
+      </c>
+      <c r="E58" s="6">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
         <v>42864</v>
       </c>
-      <c r="B56" t="s">
-        <v>51</v>
-      </c>
-      <c r="C56" s="6">
+      <c r="B59" s="6">
         <v>0.13800000000000001</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="4">
+      <c r="C59" t="str">
+        <f t="shared" si="2"/>
+        <v>Tue</v>
+      </c>
+      <c r="D59" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>May</v>
+      </c>
+      <c r="E59" s="6">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
         <v>42836</v>
       </c>
-      <c r="B57" t="s">
-        <v>52</v>
-      </c>
-      <c r="C57" s="6">
+      <c r="B60" s="6">
         <v>1.214</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="4">
+      <c r="C60" t="str">
+        <f t="shared" si="2"/>
+        <v>Tue</v>
+      </c>
+      <c r="D60" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Apr</v>
+      </c>
+      <c r="E60" s="6">
+        <f t="shared" si="6"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
         <v>42803</v>
       </c>
-      <c r="B58" t="s">
-        <v>53</v>
-      </c>
-      <c r="C58" s="6">
+      <c r="B61" s="6">
         <v>6.9000000000000006E-2</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="4">
+      <c r="C61" t="str">
+        <f t="shared" si="2"/>
+        <v>Thu</v>
+      </c>
+      <c r="D61" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Mar</v>
+      </c>
+      <c r="E61" s="6">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
         <v>42775</v>
       </c>
-      <c r="B59" t="s">
-        <v>54</v>
-      </c>
-      <c r="C59" s="6">
+      <c r="B62" s="6">
         <v>7.6999999999999999E-2</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="4">
+      <c r="C62" t="str">
+        <f t="shared" si="2"/>
+        <v>Thu</v>
+      </c>
+      <c r="D62" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Feb</v>
+      </c>
+      <c r="E62" s="6">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
         <v>42746</v>
       </c>
-      <c r="B60" t="s">
-        <v>55</v>
-      </c>
-      <c r="C60" s="6">
+      <c r="B63" s="6">
         <v>1.2330000000000001</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="4">
+      <c r="C63" t="str">
+        <f t="shared" si="2"/>
+        <v>Wed</v>
+      </c>
+      <c r="D63" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Jan</v>
+      </c>
+      <c r="E63" s="6">
+        <f t="shared" si="6"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
         <v>42713</v>
       </c>
-      <c r="B61" t="s">
-        <v>54</v>
-      </c>
-      <c r="C61" s="6">
+      <c r="B64" s="6">
         <v>7.6999999999999999E-2</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="4">
+      <c r="C64" t="str">
+        <f t="shared" si="2"/>
+        <v>Fri</v>
+      </c>
+      <c r="D64" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Dec</v>
+      </c>
+      <c r="E64" s="6">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
         <v>42683</v>
       </c>
-      <c r="B62" t="s">
-        <v>56</v>
-      </c>
-      <c r="C62" s="6">
+      <c r="B65" s="6">
         <v>0.14899999999999999</v>
       </c>
+      <c r="C65" t="str">
+        <f t="shared" si="2"/>
+        <v>Wed</v>
+      </c>
+      <c r="D65" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Nov</v>
+      </c>
+      <c r="E65" s="6">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A5:F65" xr:uid="{85ED52BC-7E95-4FEC-8B60-D730E2216244}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2616,7 +3151,7 @@
   <dimension ref="A1:F55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2627,7 +3162,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>74</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3113,7 +3648,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3129,7 +3664,7 @@
         <v>44481</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>4</v>
       </c>
       <c r="C3" s="6">
         <v>1.054</v>
@@ -3152,7 +3687,7 @@
         <v>44449</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>5</v>
       </c>
       <c r="C4" s="6">
         <v>0.16400000000000001</v>
@@ -3163,7 +3698,7 @@
         <v>44419</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="C5" s="6">
         <v>0.30599999999999999</v>
@@ -3174,7 +3709,7 @@
         <v>44390</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>7</v>
       </c>
       <c r="C6" s="6">
         <v>1.0289999999999999</v>
@@ -3185,7 +3720,7 @@
         <v>44358</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>8</v>
       </c>
       <c r="C7" s="6">
         <v>0.16800000000000001</v>
@@ -3196,7 +3731,7 @@
         <v>44328</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
+        <v>9</v>
       </c>
       <c r="C8" s="6">
         <v>0.27700000000000002</v>
@@ -3207,7 +3742,7 @@
         <v>44298</v>
       </c>
       <c r="B9" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
       <c r="C9" s="6">
         <v>0.997</v>
@@ -3218,7 +3753,7 @@
         <v>44266</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="C10">
         <v>0.09</v>
@@ -3229,7 +3764,7 @@
         <v>44238</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>11</v>
       </c>
       <c r="C11" s="6">
         <v>0.106</v>
@@ -3240,7 +3775,7 @@
         <v>44208</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
       <c r="C12" s="6">
         <v>0.97699999999999998</v>
@@ -3251,7 +3786,7 @@
         <v>44175</v>
       </c>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>13</v>
       </c>
       <c r="C13" s="6">
         <v>0.13900000000000001</v>
@@ -3262,7 +3797,7 @@
         <v>44145</v>
       </c>
       <c r="B14" t="s">
-        <v>68</v>
+        <v>14</v>
       </c>
       <c r="C14" s="6">
         <v>0.20799999999999999</v>
@@ -3273,7 +3808,7 @@
         <v>44113</v>
       </c>
       <c r="B15" t="s">
-        <v>69</v>
+        <v>15</v>
       </c>
       <c r="C15" s="6">
         <v>0.80600000000000005</v>
@@ -3284,7 +3819,7 @@
         <v>44085</v>
       </c>
       <c r="B16" t="s">
-        <v>70</v>
+        <v>16</v>
       </c>
       <c r="C16" s="6">
         <v>0.13500000000000001</v>
@@ -3295,7 +3830,7 @@
         <v>44054</v>
       </c>
       <c r="B17" t="s">
-        <v>71</v>
+        <v>17</v>
       </c>
       <c r="C17">
         <v>0.18</v>
@@ -3306,7 +3841,7 @@
         <v>44025</v>
       </c>
       <c r="B18" t="s">
-        <v>72</v>
+        <v>18</v>
       </c>
       <c r="C18" s="6">
         <v>0.79600000000000004</v>

</xml_diff>